<commit_message>
changes for 2024, add script and data for workshop
</commit_message>
<xml_diff>
--- a/metadata-file-2024-testing1.xlsx
+++ b/metadata-file-2024-testing1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yixuanwang/Documents/github/Vis24-VP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C55657-7AEE-D644-A8F9-EA94D5D57C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B7E5F2-98D2-3C43-8E3A-7551EEDF64E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19520" yWindow="-21100" windowWidth="38400" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>session_name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>award</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>time_slot</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Bayshore VI</t>
   </si>
   <si>
-    <t>v-full-1574</t>
-  </si>
-  <si>
     <t>Objective Lagrangian Vortex Cores and their Visual Representations</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Bayshore V</t>
   </si>
   <si>
-    <t>v-full-1067</t>
-  </si>
-  <si>
     <t>AdversaFlow: Visual Red Teaming for Large Language Models with Multi-Level Adversarial Flow</t>
   </si>
   <si>
@@ -188,25 +179,70 @@
   </si>
   <si>
     <t>Nils Gehlenborg, Barbora Kozlikova, Jan Byska, Qianwen Wang</t>
+  </si>
+  <si>
+    <t>cga2</t>
+  </si>
+  <si>
+    <t>thur3</t>
+  </si>
+  <si>
+    <t>2024-10-17 17:42:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-10-17 17:54:00+00:00</t>
+  </si>
+  <si>
+    <t>Francesca Samsel</t>
+  </si>
+  <si>
+    <t>fsamsel@tacc.utexas.edu</t>
+  </si>
+  <si>
+    <t>Bayshore III</t>
+  </si>
+  <si>
+    <t>v-cga-10128890</t>
+  </si>
+  <si>
+    <t>Rainbow Colormaps Are Not All Bad</t>
+  </si>
+  <si>
+    <t>Colin Ware, Maureen Stone, Danielle Albers Szafir</t>
+  </si>
+  <si>
+    <t>2024-10-17 13:42:00-04:00</t>
+  </si>
+  <si>
+    <t>2024-10-17 13:54:00-04:00</t>
+  </si>
+  <si>
+    <t>13:42</t>
+  </si>
+  <si>
+    <t>13:54</t>
+  </si>
+  <si>
+    <t>13:42-13:54</t>
+  </si>
+  <si>
+    <t>Thursday (Oct 17)</t>
+  </si>
+  <si>
+    <t>CG&amp;A-Systems, Theory, and Evaluations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -235,14 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -269,28 +298,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,278 +619,318 @@
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="21" max="21" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2"/>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
-      </c>
       <c r="T2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" t="s">
         <v>12</v>
-      </c>
-      <c r="U2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3"/>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
         <v>44</v>
       </c>
-      <c r="K3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
       <c r="N3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>37</v>
       </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
-        <v>39</v>
-      </c>
       <c r="T3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" t="s">
         <v>12</v>
-      </c>
-      <c r="U3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="7">
-        <v>2</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-    </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>9</v>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5">
+        <v>0.2</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="R5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>